<commit_message>
renamed files to be more descriptive, edited trilateral_localization.py to be more complete in tracking all circle intersection
</commit_message>
<xml_diff>
--- a/localization/coords.xlsx
+++ b/localization/coords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbb745aa252d2737/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_F25DC773A252ABDACC10480F415B4C9A5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA575AF3-D5B6-4836-B7D4-A735A8959B88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C1DC11-435B-48B5-A07A-F42C1B5C5713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,23 +153,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,508 +455,512 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="9.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.15625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1015625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.83984375" style="7"/>
+    <col min="4" max="4" width="9.1015625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.15625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.68359375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1015625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.68359375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1015625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.15625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83984375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="D2" s="8">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
         <f>SQRT((D2-$B2)^2+(E2-$C2)^2)</f>
         <v>3.1622776601683795</v>
       </c>
-      <c r="G2" s="2">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="G2" s="9">
+        <v>13</v>
+      </c>
+      <c r="H2" s="9">
+        <v>12</v>
+      </c>
+      <c r="I2" s="9">
         <f>SQRT((G2-$B2)^2+(H2-$C2)^2)</f>
         <v>9.4339811320566032</v>
       </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <v>12</v>
-      </c>
-      <c r="L2" s="3">
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <v>12</v>
+      </c>
+      <c r="L2" s="10">
         <f>SQRT((J2-$B2)^2+(K2-$C2)^2)</f>
         <v>10.63014581273465</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="D3" s="8">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
         <f t="shared" ref="F3:F12" si="0">SQRT((D3-$B3)^2+(E3-$C3)^2)</f>
         <v>8.5440037453175304</v>
       </c>
-      <c r="G3" s="2">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="G3" s="9">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9">
         <f t="shared" ref="I3:I12" si="1">SQRT((G3-$B3)^2+(H3-$C3)^2)</f>
         <v>4.2426406871192848</v>
       </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>12</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10">
+        <v>12</v>
+      </c>
+      <c r="L3" s="10">
         <f t="shared" ref="L3:L12" si="2">SQRT((J3-$B3)^2+(K3-$C3)^2)</f>
         <v>9.4868329805051381</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>8</v>
       </c>
-      <c r="D4" s="1">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="8">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
         <f t="shared" si="0"/>
         <v>7.2801098892805181</v>
       </c>
-      <c r="G4" s="2">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2">
-        <v>12</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="G4" s="9">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9">
+        <v>12</v>
+      </c>
+      <c r="I4" s="9">
         <f t="shared" si="1"/>
         <v>8.9442719099991592</v>
       </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
-        <v>12</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
+        <v>12</v>
+      </c>
+      <c r="L4" s="10">
         <f t="shared" si="2"/>
         <v>5.6568542494923806</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
         <f t="shared" si="0"/>
-        <v>12.083045973594572</v>
-      </c>
-      <c r="G5" s="2">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2">
-        <v>12</v>
-      </c>
-      <c r="I5" s="2">
+        <v>12.529964086141668</v>
+      </c>
+      <c r="G5" s="9">
+        <v>13</v>
+      </c>
+      <c r="H5" s="9">
+        <v>12</v>
+      </c>
+      <c r="I5" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3">
+        <v>12</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>12</v>
+      </c>
+      <c r="L5" s="10">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <v>-5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>-10</v>
       </c>
-      <c r="D6" s="1">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D6" s="8">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>16.278820596099706</v>
       </c>
-      <c r="G6" s="2">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2">
-        <v>12</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="G6" s="9">
+        <v>13</v>
+      </c>
+      <c r="H6" s="9">
+        <v>12</v>
+      </c>
+      <c r="I6" s="9">
         <f t="shared" si="1"/>
         <v>28.42534080710379</v>
       </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3">
-        <v>12</v>
-      </c>
-      <c r="L6" s="3">
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
+        <v>12</v>
+      </c>
+      <c r="L6" s="10">
         <f t="shared" si="2"/>
         <v>22.803508501982758</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D7" s="8">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>4.4721359549995796</v>
       </c>
-      <c r="G7" s="2">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2">
-        <v>12</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G7" s="9">
+        <v>13</v>
+      </c>
+      <c r="H7" s="9">
+        <v>12</v>
+      </c>
+      <c r="I7" s="9">
         <f t="shared" si="1"/>
         <v>10.63014581273465</v>
       </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>12</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10">
+        <v>12</v>
+      </c>
+      <c r="L7" s="10">
         <f t="shared" si="2"/>
         <v>8.0622577482985491</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>50</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>0</v>
       </c>
-      <c r="D8" s="1">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="D8" s="8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>43.011626335213137</v>
       </c>
-      <c r="G8" s="2">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2">
-        <v>12</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="G8" s="9">
+        <v>13</v>
+      </c>
+      <c r="H8" s="9">
+        <v>12</v>
+      </c>
+      <c r="I8" s="9">
         <f t="shared" si="1"/>
         <v>38.897300677553446</v>
       </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>12</v>
-      </c>
-      <c r="L8" s="3">
+      <c r="J8" s="10">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
+        <v>12</v>
+      </c>
+      <c r="L8" s="10">
         <f t="shared" si="2"/>
         <v>50.447993022517757</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="2">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2">
-        <v>12</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="G9" s="9">
+        <v>13</v>
+      </c>
+      <c r="H9" s="9">
+        <v>12</v>
+      </c>
+      <c r="I9" s="9">
         <f t="shared" si="1"/>
         <v>12.529964086141668</v>
       </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>12</v>
-      </c>
-      <c r="L9" s="3">
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
+      <c r="K9" s="10">
+        <v>12</v>
+      </c>
+      <c r="L9" s="10">
         <f t="shared" si="2"/>
         <v>12.529964086141668</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>20</v>
       </c>
-      <c r="D10" s="1">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D10" s="8">
+        <v>7</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>19.104973174542799</v>
       </c>
-      <c r="G10" s="2">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2">
-        <v>12</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="G10" s="9">
+        <v>13</v>
+      </c>
+      <c r="H10" s="9">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9">
         <f t="shared" si="1"/>
         <v>8.9442719099991592</v>
       </c>
-      <c r="J10" s="3">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3">
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10">
+        <v>12</v>
+      </c>
+      <c r="L10" s="10">
         <f t="shared" si="2"/>
         <v>11.313708498984761</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="7">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>0</v>
       </c>
-      <c r="D11" s="1">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="D11" s="8">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>7.0710678118654755</v>
       </c>
-      <c r="G11" s="2">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2">
-        <v>12</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="G11" s="9">
+        <v>13</v>
+      </c>
+      <c r="H11" s="9">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9">
         <f t="shared" si="1"/>
         <v>17.691806012954132</v>
       </c>
-      <c r="J11" s="3">
-        <v>1</v>
-      </c>
-      <c r="K11" s="3">
-        <v>12</v>
-      </c>
-      <c r="L11" s="3">
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
+      <c r="K11" s="10">
+        <v>12</v>
+      </c>
+      <c r="L11" s="10">
         <f t="shared" si="2"/>
         <v>12.041594578792296</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>12.529964086141668</v>
       </c>
-      <c r="G12" s="2">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2">
-        <v>12</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="G12" s="9">
+        <v>13</v>
+      </c>
+      <c r="H12" s="9">
+        <v>12</v>
+      </c>
+      <c r="I12" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
-      <c r="K12" s="3">
-        <v>12</v>
-      </c>
-      <c r="L12" s="3">
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
+      <c r="K12" s="10">
+        <v>12</v>
+      </c>
+      <c r="L12" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
implemented linear algebra intersections calculations for trilateration
</commit_message>
<xml_diff>
--- a/localization/coords.xlsx
+++ b/localization/coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C1DC11-435B-48B5-A07A-F42C1B5C5713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72265C6-2A09-4866-9B4F-718B4786B8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,26 +455,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.83984375" style="7"/>
-    <col min="4" max="4" width="9.1015625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.15625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.68359375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1015625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.68359375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83984375" style="7"/>
+    <col min="1" max="3" width="8.85546875" style="7"/>
+    <col min="4" max="5" width="9.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -513,7 +510,7 @@
       </c>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -554,7 +551,7 @@
         <v>10.63014581273465</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -595,7 +592,7 @@
         <v>9.4868329805051381</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -636,7 +633,7 @@
         <v>5.6568542494923806</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -678,7 +675,7 @@
       </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -719,7 +716,7 @@
         <v>22.803508501982758</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -760,7 +757,7 @@
         <v>8.0622577482985491</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -801,7 +798,7 @@
         <v>50.447993022517757</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -842,7 +839,7 @@
         <v>12.529964086141668</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -883,7 +880,7 @@
         <v>11.313708498984761</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -924,7 +921,7 @@
         <v>12.041594578792296</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -963,6 +960,47 @@
       <c r="L12" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" ref="F13" si="3">SQRT((D13-$B13)^2+(E13-$C13)^2)</f>
+        <v>12.083045973594572</v>
+      </c>
+      <c r="G13" s="9">
+        <v>13</v>
+      </c>
+      <c r="H13" s="9">
+        <v>12</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" ref="I13" si="4">SQRT((G13-$B13)^2+(H13-$C13)^2)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
+      <c r="K13" s="10">
+        <v>12</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" ref="L13" si="5">SQRT((J13-$B13)^2+(K13-$C13)^2)</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>